<commit_message>
Added filtering performance results.
</commit_message>
<xml_diff>
--- a/docs/rezultate filtre.xlsx
+++ b/docs/rezultate filtre.xlsx
@@ -372,10 +372,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H14"/>
+  <dimension ref="A1:J14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:B14"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -385,7 +385,7 @@
     <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -411,7 +411,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:10">
       <c r="A3">
         <v>3</v>
       </c>
@@ -436,8 +436,12 @@
       <c r="H3">
         <v>252</v>
       </c>
-    </row>
-    <row r="4" spans="1:8">
+      <c r="J3">
+        <f>B3/H3</f>
+        <v>0.27777777777777779</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10">
       <c r="A4">
         <v>4</v>
       </c>
@@ -462,8 +466,12 @@
       <c r="H4">
         <v>232</v>
       </c>
-    </row>
-    <row r="5" spans="1:8">
+      <c r="J4">
+        <f t="shared" ref="J4:J14" si="0">B4/H4</f>
+        <v>0.26293103448275862</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10">
       <c r="A5">
         <v>5</v>
       </c>
@@ -488,8 +496,12 @@
       <c r="H5">
         <v>273</v>
       </c>
-    </row>
-    <row r="6" spans="1:8">
+      <c r="J5">
+        <f t="shared" si="0"/>
+        <v>0.34065934065934067</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10">
       <c r="A6">
         <v>6</v>
       </c>
@@ -514,8 +526,12 @@
       <c r="H6">
         <v>298</v>
       </c>
-    </row>
-    <row r="7" spans="1:8">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>0.62416107382550334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10">
       <c r="A7">
         <v>7</v>
       </c>
@@ -540,8 +556,12 @@
       <c r="H7">
         <v>290</v>
       </c>
-    </row>
-    <row r="8" spans="1:8">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>1.3482758620689654</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10">
       <c r="A8">
         <v>8</v>
       </c>
@@ -566,8 +586,12 @@
       <c r="H8">
         <v>314</v>
       </c>
-    </row>
-    <row r="9" spans="1:8">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>2.5541401273885351</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10">
       <c r="A9">
         <v>9</v>
       </c>
@@ -592,8 +616,12 @@
       <c r="H9">
         <v>334</v>
       </c>
-    </row>
-    <row r="10" spans="1:8">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>4.6676646706586826</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10">
       <c r="A10">
         <v>10</v>
       </c>
@@ -618,8 +646,12 @@
       <c r="H10">
         <v>371</v>
       </c>
-    </row>
-    <row r="11" spans="1:8">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>7.7951482479784371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10">
       <c r="A11">
         <v>11</v>
       </c>
@@ -644,8 +676,12 @@
       <c r="H11">
         <v>407</v>
       </c>
-    </row>
-    <row r="12" spans="1:8">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>14.262899262899262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10">
       <c r="A12">
         <v>12</v>
       </c>
@@ -670,8 +706,12 @@
       <c r="H12">
         <v>492</v>
       </c>
-    </row>
-    <row r="13" spans="1:8">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>24.176829268292682</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10">
       <c r="A13">
         <v>13</v>
       </c>
@@ -696,8 +736,12 @@
       <c r="H13">
         <v>572</v>
       </c>
-    </row>
-    <row r="14" spans="1:8">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>43.566433566433567</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10">
       <c r="A14">
         <v>14</v>
       </c>
@@ -721,6 +765,10 @@
       </c>
       <c r="H14">
         <v>904</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>51.172566371681413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>